<commit_message>
added generation of soundfont textfile
</commit_message>
<xml_diff>
--- a/data/soundfont/viena_definitions_GONG_KEBYAR1.xlsx
+++ b/data/soundfont/viena_definitions_GONG_KEBYAR1.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X142"/>
+  <dimension ref="A1:AE161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1838,17 +1838,17 @@
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>REYONG BYONG OPEN</t>
+          <t>REYONG BYONG MUTED</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Reyong BYONG.wav</t>
+          <t>Reyong JET.wav</t>
         </is>
       </c>
     </row>
@@ -1856,17 +1856,17 @@
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
-          <t>REYONG BYONG ABBREVI</t>
+          <t>REYONG BYONG MUTED</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Reyong BYOT.wav</t>
+          <t>Reyong JET.wav</t>
         </is>
       </c>
     </row>
@@ -1874,17 +1874,17 @@
       <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
-          <t>REYONG TICK OPEN</t>
+          <t>REYONG BYONG MUTED</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Reyong TICK_1_PANGGUL.wav</t>
+          <t>Reyong JET.wav</t>
         </is>
       </c>
     </row>
@@ -1892,17 +1892,17 @@
       <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
-          <t>REYONG TICK_2_P OPEN</t>
+          <t>REYONG BYONG OPEN</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Reyong TICK_2_PANGGUL.wav</t>
+          <t>Reyong BYONG.wav</t>
         </is>
       </c>
     </row>
@@ -1910,17 +1910,17 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr">
         <is>
-          <t>UGAL DONG0 OPEN</t>
+          <t>REYONG BYONG OPEN</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="n">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Ugal DONG0.wav</t>
+          <t>Reyong BYONG.wav</t>
         </is>
       </c>
     </row>
@@ -1928,17 +1928,17 @@
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr">
         <is>
-          <t>UGAL DENG0 OPEN</t>
+          <t>REYONG BYONG OPEN</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="n">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Ugal DENG0.wav</t>
+          <t>Reyong BYONG.wav</t>
         </is>
       </c>
     </row>
@@ -1946,17 +1946,17 @@
       <c r="A84" t="inlineStr"/>
       <c r="B84" t="inlineStr">
         <is>
-          <t>UGAL DUNG0 OPEN</t>
+          <t>REYONG BYONG OPEN</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="n">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Ugal DUNG0.wav</t>
+          <t>Reyong BYONG.wav</t>
         </is>
       </c>
     </row>
@@ -1964,17 +1964,17 @@
       <c r="A85" t="inlineStr"/>
       <c r="B85" t="inlineStr">
         <is>
-          <t>UGAL DANG0 OPEN</t>
+          <t>REYONG BYONG ABBREVI</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="n">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Ugal DANG0.wav</t>
+          <t>Reyong BYOT.wav</t>
         </is>
       </c>
     </row>
@@ -1982,17 +1982,17 @@
       <c r="A86" t="inlineStr"/>
       <c r="B86" t="inlineStr">
         <is>
-          <t>UGAL DING1 OPEN</t>
+          <t>REYONG BYONG ABBREVI</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Ugal DING1.wav</t>
+          <t>Reyong BYOT.wav</t>
         </is>
       </c>
     </row>
@@ -2000,17 +2000,17 @@
       <c r="A87" t="inlineStr"/>
       <c r="B87" t="inlineStr">
         <is>
-          <t>UGAL DONG1 OPEN</t>
+          <t>REYONG BYONG ABBREVI</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="n">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Ugal DONG1.wav</t>
+          <t>Reyong BYOT.wav</t>
         </is>
       </c>
     </row>
@@ -2018,17 +2018,17 @@
       <c r="A88" t="inlineStr"/>
       <c r="B88" t="inlineStr">
         <is>
-          <t>UGAL DENG1 OPEN</t>
+          <t>REYONG BYONG ABBREVI</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="n">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Ugal DENG1.wav</t>
+          <t>Reyong BYOT.wav</t>
         </is>
       </c>
     </row>
@@ -2036,17 +2036,17 @@
       <c r="A89" t="inlineStr"/>
       <c r="B89" t="inlineStr">
         <is>
-          <t>UGAL DUNG1 OPEN</t>
+          <t>REYONG TICK OPEN</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="n">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Ugal DUNG1.wav</t>
+          <t>Reyong TICK_1_PANGGUL.wav</t>
         </is>
       </c>
     </row>
@@ -2054,17 +2054,17 @@
       <c r="A90" t="inlineStr"/>
       <c r="B90" t="inlineStr">
         <is>
-          <t>UGAL DANG1 OPEN</t>
+          <t>REYONG TICK_2_P OPEN</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="n">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Ugal DANG1.wav</t>
+          <t>Reyong TICK_2_PANGGUL.wav</t>
         </is>
       </c>
     </row>
@@ -2072,55 +2072,71 @@
       <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr">
         <is>
-          <t>UGAL DING2 OPEN</t>
+          <t>UGAL DONG0 OPEN</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="n">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Ugal DING2.wav</t>
+          <t>Ugal DONG0.wav</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>Search paths:</t>
-        </is>
-      </c>
+      <c r="A92" t="inlineStr"/>
       <c r="B92" t="inlineStr">
         <is>
-          <t>C:\Users\marcp\Documents\administratie\_VRIJETIJD_REIZEN\Scripts-Programmas\PythonProjects\gamelan-notation\data\samples</t>
+          <t>UGAL DONG0 MUTED</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>95</v>
+      </c>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Ugal DONG0.wav</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="n"/>
-      <c r="B93" s="2" t="n"/>
-      <c r="C93" s="2" t="n"/>
-      <c r="D93" s="2" t="n"/>
-      <c r="E93" s="2" t="n"/>
-      <c r="F93" s="2" t="n"/>
-      <c r="G93" s="2" t="n"/>
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>UGAL DENG0 OPEN</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>96</v>
+      </c>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Ugal DENG0.wav</t>
+        </is>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>Instruments</t>
-        </is>
-      </c>
-      <c r="B94" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C94" s="1" t="inlineStr">
-        <is>
-          <t>Generators</t>
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>UGAL DENG0 MUTED</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>96</v>
+      </c>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Ugal DENG0.wav</t>
         </is>
       </c>
     </row>
@@ -2128,672 +2144,372 @@
       <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CALUNG</t>
+          <t>UGAL DUNG0 OPEN</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>97</v>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Ugal DUNG0.wav</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" s="1" t="inlineStr">
-        <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>CALUNG DING1 OPEN</t>
-        </is>
-      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>UGAL DUNG0 MUTED</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="n">
+        <v>97</v>
+      </c>
+      <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
-          <t>CALUNG DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>CALUNG DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>CALUNG DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>CALUNG DANG1 OPEN</t>
+          <t>Ugal DUNG0.wav</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" s="1" t="inlineStr">
-        <is>
-          <t>Key Range</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>25-25</t>
-        </is>
-      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>UGAL DANG0 OPEN</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="n">
+        <v>98</v>
+      </c>
+      <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr">
         <is>
-          <t>26-26</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>27-27</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>28-28</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>29-29</t>
+          <t>Ugal DANG0.wav</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>25</v>
-      </c>
-      <c r="F98" t="n">
-        <v>26</v>
-      </c>
-      <c r="G98" t="n">
-        <v>27</v>
-      </c>
-      <c r="H98" t="n">
-        <v>28</v>
-      </c>
-      <c r="I98" t="n">
-        <v>29</v>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>UGAL DANG0 MUTED</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>98</v>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Ugal DANG0.wav</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CENGCENG</t>
+          <t>UGAL DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="n">
+        <v>99</v>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Ugal DING1.wav</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" s="1" t="inlineStr">
-        <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>CENGCENG OPEN OPEN</t>
-        </is>
-      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>UGAL DING1 MUTED</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="n">
+        <v>99</v>
+      </c>
+      <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr">
         <is>
-          <t>CENGCENG MUTED OPEN</t>
+          <t>Ugal DING1.wav</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr"/>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" s="1" t="inlineStr">
-        <is>
-          <t>Key Range</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>5-5</t>
-        </is>
-      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>UGAL DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="n">
+        <v>100</v>
+      </c>
+      <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>6-6</t>
+          <t>Ugal DONG1.wav</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr"/>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="n">
-        <v>5</v>
-      </c>
-      <c r="F102" t="n">
-        <v>6</v>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>UGAL DONG1 MUTED</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="n">
+        <v>100</v>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Ugal DONG1.wav</t>
+        </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
       <c r="B103" t="inlineStr">
         <is>
-          <t>GONGS</t>
+          <t>UGAL DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="n">
+        <v>101</v>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Ugal DENG1.wav</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" s="1" t="inlineStr">
-        <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>GONGS GIR OPEN</t>
-        </is>
-      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>UGAL DENG1 MUTED</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="n">
+        <v>101</v>
+      </c>
+      <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr">
         <is>
-          <t>GONGS PUR OPEN</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>GONGS TONG OPEN</t>
+          <t>Ugal DENG1.wav</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr"/>
-      <c r="B105" t="inlineStr"/>
-      <c r="C105" s="1" t="inlineStr">
-        <is>
-          <t>Key Range</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>1-1</t>
-        </is>
-      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>UGAL DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="n">
+        <v>102</v>
+      </c>
+      <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2-2</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>3-3</t>
+          <t>Ugal DUNG1.wav</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="n">
-        <v>1</v>
-      </c>
-      <c r="F106" t="n">
-        <v>2</v>
-      </c>
-      <c r="G106" t="n">
-        <v>3</v>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>UGAL DUNG1 MUTED</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="n">
+        <v>102</v>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Ugal DUNG1.wav</t>
+        </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr"/>
       <c r="B107" t="inlineStr">
         <is>
-          <t>JEGOGAN</t>
+          <t>UGAL DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="n">
+        <v>103</v>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Ugal DANG1.wav</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr"/>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" s="1" t="inlineStr">
-        <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>JEGOGAN DING1 OPEN</t>
-        </is>
-      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>UGAL DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>103</v>
+      </c>
+      <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr">
         <is>
-          <t>JEGOGAN DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>JEGOGAN DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>JEGOGAN DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>JEGOGAN DANG1 OPEN</t>
+          <t>Ugal DANG1.wav</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr"/>
-      <c r="B109" t="inlineStr"/>
-      <c r="C109" s="1" t="inlineStr">
-        <is>
-          <t>Key Range</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>20-20</t>
-        </is>
-      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>UGAL DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="n">
+        <v>104</v>
+      </c>
+      <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr">
         <is>
-          <t>21-21</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>22-22</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>23-23</t>
-        </is>
-      </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>24-24</t>
+          <t>Ugal DING2.wav</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr"/>
-      <c r="B110" t="inlineStr"/>
-      <c r="C110" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr"/>
-      <c r="E110" t="n">
-        <v>20</v>
-      </c>
-      <c r="F110" t="n">
-        <v>21</v>
-      </c>
-      <c r="G110" t="n">
-        <v>22</v>
-      </c>
-      <c r="H110" t="n">
-        <v>23</v>
-      </c>
-      <c r="I110" t="n">
-        <v>24</v>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>UGAL DING2 MUTED</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="n">
+        <v>104</v>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Ugal DING2.wav</t>
+        </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr"/>
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Search paths:</t>
+        </is>
+      </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>KANTILAN</t>
+          <t>C:\Users\marcp\Documents\administratie\_VRIJETIJD_REIZEN\Scripts-Programmas\PythonProjects\gamelan-notation\data\samples</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr"/>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" s="1" t="inlineStr">
-        <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG0 OPEN</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG0 MUTED</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG0 OPEN</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG0 MUTED</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG0 OPEN</t>
-        </is>
-      </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG0 MUTED</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG0 OPEN</t>
-        </is>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG0 MUTED</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>KANTILAN DING1 OPEN</t>
-        </is>
-      </c>
-      <c r="N112" t="inlineStr">
-        <is>
-          <t>KANTILAN DING1 MUTED</t>
-        </is>
-      </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="P112" t="inlineStr">
-        <is>
-          <t>KANTILAN DONG1 MUTED</t>
-        </is>
-      </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="R112" t="inlineStr">
-        <is>
-          <t>KANTILAN DENG1 MUTED</t>
-        </is>
-      </c>
-      <c r="S112" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="T112" t="inlineStr">
-        <is>
-          <t>KANTILAN DUNG1 MUTED</t>
-        </is>
-      </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG1 OPEN</t>
-        </is>
-      </c>
-      <c r="V112" t="inlineStr">
-        <is>
-          <t>KANTILAN DANG1 MUTED</t>
-        </is>
-      </c>
-      <c r="W112" t="inlineStr">
-        <is>
-          <t>KANTILAN DING2 OPEN</t>
-        </is>
-      </c>
-      <c r="X112" t="inlineStr">
-        <is>
-          <t>KANTILAN DING2 MUTED</t>
-        </is>
-      </c>
+      <c r="A112" s="2" t="n"/>
+      <c r="B112" s="2" t="n"/>
+      <c r="C112" s="2" t="n"/>
+      <c r="D112" s="2" t="n"/>
+      <c r="E112" s="2" t="n"/>
+      <c r="F112" s="2" t="n"/>
+      <c r="G112" s="2" t="n"/>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Instruments</t>
+        </is>
+      </c>
+      <c r="B113" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
       <c r="C113" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>55-55</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>56-56</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>57-57</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>58-58</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>59-59</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>60-60</t>
-        </is>
-      </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>61-61</t>
-        </is>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>62-62</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>63-63</t>
-        </is>
-      </c>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>64-64</t>
-        </is>
-      </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>65-65</t>
-        </is>
-      </c>
-      <c r="P113" t="inlineStr">
-        <is>
-          <t>66-66</t>
-        </is>
-      </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>67-67</t>
-        </is>
-      </c>
-      <c r="R113" t="inlineStr">
-        <is>
-          <t>68-68</t>
-        </is>
-      </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>69-69</t>
-        </is>
-      </c>
-      <c r="T113" t="inlineStr">
-        <is>
-          <t>70-70</t>
-        </is>
-      </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>71-71</t>
-        </is>
-      </c>
-      <c r="V113" t="inlineStr">
-        <is>
-          <t>72-72</t>
-        </is>
-      </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>73-73</t>
-        </is>
-      </c>
-      <c r="X113" t="inlineStr">
-        <is>
-          <t>74-74</t>
+          <t>Generators</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr"/>
-      <c r="E114" t="n">
-        <v>55</v>
-      </c>
-      <c r="F114" t="n">
-        <v>56</v>
-      </c>
-      <c r="G114" t="n">
-        <v>57</v>
-      </c>
-      <c r="H114" t="n">
-        <v>58</v>
-      </c>
-      <c r="I114" t="n">
-        <v>59</v>
-      </c>
-      <c r="J114" t="n">
-        <v>60</v>
-      </c>
-      <c r="K114" t="n">
-        <v>61</v>
-      </c>
-      <c r="L114" t="n">
-        <v>62</v>
-      </c>
-      <c r="M114" t="n">
-        <v>63</v>
-      </c>
-      <c r="N114" t="n">
-        <v>64</v>
-      </c>
-      <c r="O114" t="n">
-        <v>65</v>
-      </c>
-      <c r="P114" t="n">
-        <v>66</v>
-      </c>
-      <c r="Q114" t="n">
-        <v>67</v>
-      </c>
-      <c r="R114" t="n">
-        <v>68</v>
-      </c>
-      <c r="S114" t="n">
-        <v>69</v>
-      </c>
-      <c r="T114" t="n">
-        <v>70</v>
-      </c>
-      <c r="U114" t="n">
-        <v>71</v>
-      </c>
-      <c r="V114" t="n">
-        <v>72</v>
-      </c>
-      <c r="W114" t="n">
-        <v>73</v>
-      </c>
-      <c r="X114" t="n">
-        <v>74</v>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>CALUNG</t>
+        </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>KEMPLI</t>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>CALUNG DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>CALUNG DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>CALUNG DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>CALUNG DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>CALUNG DANG1 OPEN</t>
         </is>
       </c>
     </row>
@@ -2802,17 +2518,33 @@
       <c r="B116" t="inlineStr"/>
       <c r="C116" s="1" t="inlineStr">
         <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t>KEMPLI TICK OPEN</t>
+          <t>25-25</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>26-26</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>27-27</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>28-28</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>29-29</t>
         </is>
       </c>
     </row>
@@ -2821,34 +2553,55 @@
       <c r="B117" t="inlineStr"/>
       <c r="C117" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
+          <t>Root Key</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>4-4</t>
-        </is>
+      <c r="E117" t="n">
+        <v>25</v>
+      </c>
+      <c r="F117" t="n">
+        <v>26</v>
+      </c>
+      <c r="G117" t="n">
+        <v>27</v>
+      </c>
+      <c r="H117" t="n">
+        <v>28</v>
+      </c>
+      <c r="I117" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr"/>
-      <c r="E118" t="n">
-        <v>4</v>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>CENGCENG</t>
+        </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>KENDANG</t>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>CENGCENG OPEN OPEN</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>CENGCENG MUTED OPEN</t>
         </is>
       </c>
     </row>
@@ -2857,42 +2610,18 @@
       <c r="B120" t="inlineStr"/>
       <c r="C120" s="1" t="inlineStr">
         <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
-          <t>KENDANG KA OPEN</t>
+          <t>5-5</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>KENDANG PAK OPEN</t>
-        </is>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>KENDANG DE OPEN</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>KENDANG TUT OPEN</t>
-        </is>
-      </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>KENDANG JU OPEN</t>
-        </is>
-      </c>
-      <c r="J120" t="inlineStr">
-        <is>
-          <t>KENDANG KUNG OPEN</t>
+          <t>6-6</t>
         </is>
       </c>
     </row>
@@ -2901,74 +2630,51 @@
       <c r="B121" t="inlineStr"/>
       <c r="C121" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
+          <t>Root Key</t>
         </is>
       </c>
       <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>7-7</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>8-8</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>9-9</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>10-10</t>
-        </is>
-      </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>11-11</t>
-        </is>
-      </c>
-      <c r="J121" t="inlineStr">
-        <is>
-          <t>12-12</t>
-        </is>
+      <c r="E121" t="n">
+        <v>5</v>
+      </c>
+      <c r="F121" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr"/>
-      <c r="E122" t="n">
-        <v>7</v>
-      </c>
-      <c r="F122" t="n">
-        <v>8</v>
-      </c>
-      <c r="G122" t="n">
-        <v>9</v>
-      </c>
-      <c r="H122" t="n">
-        <v>10</v>
-      </c>
-      <c r="I122" t="n">
-        <v>11</v>
-      </c>
-      <c r="J122" t="n">
-        <v>12</v>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>GONGS</t>
+        </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>PEMADE</t>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>GONGS GIR OPEN</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>GONGS PUR OPEN</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>GONGS TONG OPEN</t>
         </is>
       </c>
     </row>
@@ -2977,112 +2683,23 @@
       <c r="B124" t="inlineStr"/>
       <c r="C124" s="1" t="inlineStr">
         <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr">
         <is>
-          <t>PEMADE DONG0 OPEN</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>PEMADE DONG0 MUTED</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>PEMADE DENG0 OPEN</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>PEMADE DENG0 MUTED</t>
-        </is>
-      </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG0 OPEN</t>
-        </is>
-      </c>
-      <c r="J124" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG0 MUTED</t>
-        </is>
-      </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>PEMADE DANG0 OPEN</t>
-        </is>
-      </c>
-      <c r="L124" t="inlineStr">
-        <is>
-          <t>PEMADE DANG0 MUTED</t>
-        </is>
-      </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>PEMADE DING1 OPEN</t>
-        </is>
-      </c>
-      <c r="N124" t="inlineStr">
-        <is>
-          <t>PEMADE DING1 MUTED</t>
-        </is>
-      </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>PEMADE DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="P124" t="inlineStr">
-        <is>
-          <t>PEMADE DONG1 MUTED</t>
-        </is>
-      </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>PEMADE DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="R124" t="inlineStr">
-        <is>
-          <t>PEMADE DENG1 MUTED</t>
-        </is>
-      </c>
-      <c r="S124" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="T124" t="inlineStr">
-        <is>
-          <t>PEMADE DUNG1 MUTED</t>
-        </is>
-      </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>PEMADE DANG1 OPEN</t>
-        </is>
-      </c>
-      <c r="V124" t="inlineStr">
-        <is>
-          <t>PEMADE DANG1 MUTED</t>
-        </is>
-      </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>PEMADE DING2 OPEN</t>
-        </is>
-      </c>
-      <c r="X124" t="inlineStr">
-        <is>
-          <t>PEMADE DING2 MUTED</t>
+          <t>3-3</t>
         </is>
       </c>
     </row>
@@ -3091,186 +2708,64 @@
       <c r="B125" t="inlineStr"/>
       <c r="C125" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
+          <t>Root Key</t>
         </is>
       </c>
       <c r="D125" t="inlineStr"/>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>75-75</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>76-76</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>77-77</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t>78-78</t>
-        </is>
-      </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>79-79</t>
-        </is>
-      </c>
-      <c r="J125" t="inlineStr">
-        <is>
-          <t>80-80</t>
-        </is>
-      </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>81-81</t>
-        </is>
-      </c>
-      <c r="L125" t="inlineStr">
-        <is>
-          <t>82-82</t>
-        </is>
-      </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>83-83</t>
-        </is>
-      </c>
-      <c r="N125" t="inlineStr">
-        <is>
-          <t>84-84</t>
-        </is>
-      </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>85-85</t>
-        </is>
-      </c>
-      <c r="P125" t="inlineStr">
-        <is>
-          <t>86-86</t>
-        </is>
-      </c>
-      <c r="Q125" t="inlineStr">
-        <is>
-          <t>87-87</t>
-        </is>
-      </c>
-      <c r="R125" t="inlineStr">
-        <is>
-          <t>88-88</t>
-        </is>
-      </c>
-      <c r="S125" t="inlineStr">
-        <is>
-          <t>89-89</t>
-        </is>
-      </c>
-      <c r="T125" t="inlineStr">
-        <is>
-          <t>90-90</t>
-        </is>
-      </c>
-      <c r="U125" t="inlineStr">
-        <is>
-          <t>91-91</t>
-        </is>
-      </c>
-      <c r="V125" t="inlineStr">
-        <is>
-          <t>92-92</t>
-        </is>
-      </c>
-      <c r="W125" t="inlineStr">
-        <is>
-          <t>93-93</t>
-        </is>
-      </c>
-      <c r="X125" t="inlineStr">
-        <is>
-          <t>94-94</t>
-        </is>
+      <c r="E125" t="n">
+        <v>1</v>
+      </c>
+      <c r="F125" t="n">
+        <v>2</v>
+      </c>
+      <c r="G125" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr"/>
-      <c r="E126" t="n">
-        <v>75</v>
-      </c>
-      <c r="F126" t="n">
-        <v>76</v>
-      </c>
-      <c r="G126" t="n">
-        <v>77</v>
-      </c>
-      <c r="H126" t="n">
-        <v>78</v>
-      </c>
-      <c r="I126" t="n">
-        <v>79</v>
-      </c>
-      <c r="J126" t="n">
-        <v>80</v>
-      </c>
-      <c r="K126" t="n">
-        <v>81</v>
-      </c>
-      <c r="L126" t="n">
-        <v>82</v>
-      </c>
-      <c r="M126" t="n">
-        <v>83</v>
-      </c>
-      <c r="N126" t="n">
-        <v>84</v>
-      </c>
-      <c r="O126" t="n">
-        <v>85</v>
-      </c>
-      <c r="P126" t="n">
-        <v>86</v>
-      </c>
-      <c r="Q126" t="n">
-        <v>87</v>
-      </c>
-      <c r="R126" t="n">
-        <v>88</v>
-      </c>
-      <c r="S126" t="n">
-        <v>89</v>
-      </c>
-      <c r="T126" t="n">
-        <v>90</v>
-      </c>
-      <c r="U126" t="n">
-        <v>91</v>
-      </c>
-      <c r="V126" t="n">
-        <v>92</v>
-      </c>
-      <c r="W126" t="n">
-        <v>93</v>
-      </c>
-      <c r="X126" t="n">
-        <v>94</v>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>JEGOGAN</t>
+        </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>REYONG</t>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>JEGOGAN DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>JEGOGAN DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>JEGOGAN DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>JEGOGAN DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>JEGOGAN DANG1 OPEN</t>
         </is>
       </c>
     </row>
@@ -3279,102 +2774,33 @@
       <c r="B128" t="inlineStr"/>
       <c r="C128" s="1" t="inlineStr">
         <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr">
         <is>
-          <t>REYONG DENG0 OPEN</t>
+          <t>20-20</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>REYONG DUNG0 OPEN</t>
+          <t>21-21</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>REYONG DANG0 OPEN</t>
+          <t>22-22</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>REYONG DING1 OPEN</t>
+          <t>23-23</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>REYONG DENGDIN0 OPEN</t>
-        </is>
-      </c>
-      <c r="J128" t="inlineStr">
-        <is>
-          <t>REYONG DONG1 OPEN</t>
-        </is>
-      </c>
-      <c r="K128" t="inlineStr">
-        <is>
-          <t>REYONG DENG1 OPEN</t>
-        </is>
-      </c>
-      <c r="L128" t="inlineStr">
-        <is>
-          <t>REYONG DUNG1 OPEN</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>REYONG DANG1 OPEN</t>
-        </is>
-      </c>
-      <c r="N128" t="inlineStr">
-        <is>
-          <t>REYONG DING2 OPEN</t>
-        </is>
-      </c>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>REYONG DONG2 OPEN</t>
-        </is>
-      </c>
-      <c r="P128" t="inlineStr">
-        <is>
-          <t>REYONG DENG2 OPEN</t>
-        </is>
-      </c>
-      <c r="Q128" t="inlineStr">
-        <is>
-          <t>REYONG DUNG2 OPEN</t>
-        </is>
-      </c>
-      <c r="R128" t="inlineStr">
-        <is>
-          <t>REYONG BYONG MUTED</t>
-        </is>
-      </c>
-      <c r="S128" t="inlineStr">
-        <is>
-          <t>REYONG BYONG OPEN</t>
-        </is>
-      </c>
-      <c r="T128" t="inlineStr">
-        <is>
-          <t>REYONG BYONG ABBREVI</t>
-        </is>
-      </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>REYONG TICK OPEN</t>
-        </is>
-      </c>
-      <c r="V128" t="inlineStr">
-        <is>
-          <t>REYONG TICK_2_P OPEN</t>
+          <t>24-24</t>
         </is>
       </c>
     </row>
@@ -3383,170 +2809,145 @@
       <c r="B129" t="inlineStr"/>
       <c r="C129" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
+          <t>Root Key</t>
         </is>
       </c>
       <c r="D129" t="inlineStr"/>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>30-30</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>31-31</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>32-32</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
-        <is>
-          <t>33-33</t>
-        </is>
-      </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>34-34</t>
-        </is>
-      </c>
-      <c r="J129" t="inlineStr">
-        <is>
-          <t>35-35</t>
-        </is>
-      </c>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>36-36</t>
-        </is>
-      </c>
-      <c r="L129" t="inlineStr">
-        <is>
-          <t>37-37</t>
-        </is>
-      </c>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>38-38</t>
-        </is>
-      </c>
-      <c r="N129" t="inlineStr">
-        <is>
-          <t>39-39</t>
-        </is>
-      </c>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>40-40</t>
-        </is>
-      </c>
-      <c r="P129" t="inlineStr">
-        <is>
-          <t>41-41</t>
-        </is>
-      </c>
-      <c r="Q129" t="inlineStr">
-        <is>
-          <t>42-42</t>
-        </is>
-      </c>
-      <c r="R129" t="inlineStr">
-        <is>
-          <t>43-43</t>
-        </is>
-      </c>
-      <c r="S129" t="inlineStr">
-        <is>
-          <t>44-44</t>
-        </is>
-      </c>
-      <c r="T129" t="inlineStr">
-        <is>
-          <t>45-45</t>
-        </is>
-      </c>
-      <c r="U129" t="inlineStr">
-        <is>
-          <t>46-46</t>
-        </is>
-      </c>
-      <c r="V129" t="inlineStr">
-        <is>
-          <t>47-47</t>
-        </is>
+      <c r="E129" t="n">
+        <v>20</v>
+      </c>
+      <c r="F129" t="n">
+        <v>21</v>
+      </c>
+      <c r="G129" t="n">
+        <v>22</v>
+      </c>
+      <c r="H129" t="n">
+        <v>23</v>
+      </c>
+      <c r="I129" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr"/>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr"/>
-      <c r="E130" t="n">
-        <v>30</v>
-      </c>
-      <c r="F130" t="n">
-        <v>31</v>
-      </c>
-      <c r="G130" t="n">
-        <v>32</v>
-      </c>
-      <c r="H130" t="n">
-        <v>33</v>
-      </c>
-      <c r="I130" t="n">
-        <v>34</v>
-      </c>
-      <c r="J130" t="n">
-        <v>35</v>
-      </c>
-      <c r="K130" t="n">
-        <v>36</v>
-      </c>
-      <c r="L130" t="n">
-        <v>37</v>
-      </c>
-      <c r="M130" t="n">
-        <v>38</v>
-      </c>
-      <c r="N130" t="n">
-        <v>39</v>
-      </c>
-      <c r="O130" t="n">
-        <v>40</v>
-      </c>
-      <c r="P130" t="n">
-        <v>41</v>
-      </c>
-      <c r="Q130" t="n">
-        <v>42</v>
-      </c>
-      <c r="R130" t="n">
-        <v>43</v>
-      </c>
-      <c r="S130" t="n">
-        <v>44</v>
-      </c>
-      <c r="T130" t="n">
-        <v>45</v>
-      </c>
-      <c r="U130" t="n">
-        <v>46</v>
-      </c>
-      <c r="V130" t="n">
-        <v>47</v>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>KANTILAN</t>
+        </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr"/>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>UGAL</t>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG0 OPEN</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG0 MUTED</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG0 OPEN</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG0 MUTED</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG0 OPEN</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG0 MUTED</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG0 OPEN</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG0 MUTED</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>KANTILAN DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>KANTILAN DING1 MUTED</t>
+        </is>
+      </c>
+      <c r="O131" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>KANTILAN DONG1 MUTED</t>
+        </is>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>KANTILAN DENG1 MUTED</t>
+        </is>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="T131" t="inlineStr">
+        <is>
+          <t>KANTILAN DUNG1 MUTED</t>
+        </is>
+      </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="V131" t="inlineStr">
+        <is>
+          <t>KANTILAN DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="W131" t="inlineStr">
+        <is>
+          <t>KANTILAN DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="X131" t="inlineStr">
+        <is>
+          <t>KANTILAN DING2 MUTED</t>
         </is>
       </c>
     </row>
@@ -3555,62 +2956,108 @@
       <c r="B132" t="inlineStr"/>
       <c r="C132" s="1" t="inlineStr">
         <is>
-          <t>Sample name</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr">
         <is>
-          <t>UGAL DONG0 OPEN</t>
+          <t>55-55</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>UGAL DENG0 OPEN</t>
+          <t>56-56</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>UGAL DUNG0 OPEN</t>
+          <t>57-57</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>UGAL DANG0 OPEN</t>
+          <t>58-58</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>UGAL DING1 OPEN</t>
+          <t>59-59</t>
         </is>
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>UGAL DONG1 OPEN</t>
+          <t>60-60</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>UGAL DENG1 OPEN</t>
+          <t>61-61</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>UGAL DUNG1 OPEN</t>
+          <t>62-62</t>
         </is>
       </c>
       <c r="M132" t="inlineStr">
         <is>
-          <t>UGAL DANG1 OPEN</t>
+          <t>63-63</t>
         </is>
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>UGAL DING2 OPEN</t>
+          <t>64-64</t>
+        </is>
+      </c>
+      <c r="O132" t="inlineStr">
+        <is>
+          <t>65-65</t>
+        </is>
+      </c>
+      <c r="P132" t="inlineStr">
+        <is>
+          <t>66-66</t>
+        </is>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>67-67</t>
+        </is>
+      </c>
+      <c r="R132" t="inlineStr">
+        <is>
+          <t>68-68</t>
+        </is>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>69-69</t>
+        </is>
+      </c>
+      <c r="T132" t="inlineStr">
+        <is>
+          <t>70-70</t>
+        </is>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>71-71</t>
+        </is>
+      </c>
+      <c r="V132" t="inlineStr">
+        <is>
+          <t>72-72</t>
+        </is>
+      </c>
+      <c r="W132" t="inlineStr">
+        <is>
+          <t>73-73</t>
+        </is>
+      </c>
+      <c r="X132" t="inlineStr">
+        <is>
+          <t>74-74</t>
         </is>
       </c>
     </row>
@@ -3619,209 +3066,176 @@
       <c r="B133" t="inlineStr"/>
       <c r="C133" s="1" t="inlineStr">
         <is>
-          <t>Key Range</t>
+          <t>Root Key</t>
         </is>
       </c>
       <c r="D133" t="inlineStr"/>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>95-95</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>96-96</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>97-97</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>98-98</t>
-        </is>
-      </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>99-99</t>
-        </is>
-      </c>
-      <c r="J133" t="inlineStr">
-        <is>
-          <t>100-100</t>
-        </is>
-      </c>
-      <c r="K133" t="inlineStr">
-        <is>
-          <t>101-101</t>
-        </is>
-      </c>
-      <c r="L133" t="inlineStr">
-        <is>
-          <t>102-102</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr">
-        <is>
-          <t>103-103</t>
-        </is>
-      </c>
-      <c r="N133" t="inlineStr">
-        <is>
-          <t>104-104</t>
-        </is>
+      <c r="E133" t="n">
+        <v>55</v>
+      </c>
+      <c r="F133" t="n">
+        <v>56</v>
+      </c>
+      <c r="G133" t="n">
+        <v>57</v>
+      </c>
+      <c r="H133" t="n">
+        <v>58</v>
+      </c>
+      <c r="I133" t="n">
+        <v>59</v>
+      </c>
+      <c r="J133" t="n">
+        <v>60</v>
+      </c>
+      <c r="K133" t="n">
+        <v>61</v>
+      </c>
+      <c r="L133" t="n">
+        <v>62</v>
+      </c>
+      <c r="M133" t="n">
+        <v>63</v>
+      </c>
+      <c r="N133" t="n">
+        <v>64</v>
+      </c>
+      <c r="O133" t="n">
+        <v>65</v>
+      </c>
+      <c r="P133" t="n">
+        <v>66</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>67</v>
+      </c>
+      <c r="R133" t="n">
+        <v>68</v>
+      </c>
+      <c r="S133" t="n">
+        <v>69</v>
+      </c>
+      <c r="T133" t="n">
+        <v>70</v>
+      </c>
+      <c r="U133" t="n">
+        <v>71</v>
+      </c>
+      <c r="V133" t="n">
+        <v>72</v>
+      </c>
+      <c r="W133" t="n">
+        <v>73</v>
+      </c>
+      <c r="X133" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr"/>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" s="1" t="inlineStr">
-        <is>
-          <t>Root Key</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="n">
-        <v>95</v>
-      </c>
-      <c r="F134" t="n">
-        <v>96</v>
-      </c>
-      <c r="G134" t="n">
-        <v>97</v>
-      </c>
-      <c r="H134" t="n">
-        <v>98</v>
-      </c>
-      <c r="I134" t="n">
-        <v>99</v>
-      </c>
-      <c r="J134" t="n">
-        <v>100</v>
-      </c>
-      <c r="K134" t="n">
-        <v>101</v>
-      </c>
-      <c r="L134" t="n">
-        <v>102</v>
-      </c>
-      <c r="M134" t="n">
-        <v>103</v>
-      </c>
-      <c r="N134" t="n">
-        <v>104</v>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>KEMPLI</t>
+        </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="n"/>
-      <c r="B135" s="2" t="n"/>
-      <c r="C135" s="2" t="n"/>
-      <c r="D135" s="2" t="n"/>
-      <c r="E135" s="2" t="n"/>
-      <c r="F135" s="2" t="n"/>
-      <c r="G135" s="2" t="n"/>
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>KEMPLI TICK OPEN</t>
+        </is>
+      </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="inlineStr">
-        <is>
-          <t>Presets</t>
-        </is>
-      </c>
-      <c r="B136" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr"/>
       <c r="C136" s="1" t="inlineStr">
         <is>
-          <t>Generators</t>
-        </is>
-      </c>
-      <c r="D136" s="1" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="E136" s="1" t="inlineStr">
-        <is>
-          <t>Preset</t>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>4-4</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr"/>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Gong Kebyar melodic</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr"/>
-      <c r="D137" t="n">
-        <v>0</v>
-      </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" s="1" t="inlineStr">
+        <is>
+          <t>Root Key</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr"/>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr"/>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" s="1" t="inlineStr">
-        <is>
-          <t>Instrument name</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Global</t>
-        </is>
-      </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>JEGOGAN</t>
-        </is>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>CALUNG</t>
-        </is>
-      </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>PEMADE</t>
-        </is>
-      </c>
-      <c r="H138" t="inlineStr">
-        <is>
-          <t>KANTILAN</t>
-        </is>
-      </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>UGAL</t>
-        </is>
-      </c>
-      <c r="J138" t="inlineStr">
-        <is>
-          <t>REYONG</t>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>KENDANG</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr"/>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Gong Kebyar percussion</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="n">
-        <v>128</v>
-      </c>
-      <c r="E139" t="n">
-        <v>0</v>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>KENDANG KA OPEN</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>KENDANG PAK OPEN</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>KENDANG DE OPEN</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>KENDANG TUT OPEN</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>KENDANG JU OPEN</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>KENDANG KUNG OPEN</t>
+        </is>
       </c>
     </row>
     <row r="140">
@@ -3829,50 +3243,1225 @@
       <c r="B140" t="inlineStr"/>
       <c r="C140" s="1" t="inlineStr">
         <is>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>7-7</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>8-8</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>9-9</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>10-10</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>11-11</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>12-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" s="1" t="inlineStr">
+        <is>
+          <t>Root Key</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="n">
+        <v>7</v>
+      </c>
+      <c r="F141" t="n">
+        <v>8</v>
+      </c>
+      <c r="G141" t="n">
+        <v>9</v>
+      </c>
+      <c r="H141" t="n">
+        <v>10</v>
+      </c>
+      <c r="I141" t="n">
+        <v>11</v>
+      </c>
+      <c r="J141" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>PEMADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>PEMADE DONG0 OPEN</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>PEMADE DONG0 MUTED</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>PEMADE DENG0 OPEN</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>PEMADE DENG0 MUTED</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>PEMADE DUNG0 OPEN</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>PEMADE DUNG0 MUTED</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>PEMADE DANG0 OPEN</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>PEMADE DANG0 MUTED</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>PEMADE DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>PEMADE DING1 MUTED</t>
+        </is>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>PEMADE DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="P143" t="inlineStr">
+        <is>
+          <t>PEMADE DONG1 MUTED</t>
+        </is>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>PEMADE DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="R143" t="inlineStr">
+        <is>
+          <t>PEMADE DENG1 MUTED</t>
+        </is>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>PEMADE DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="T143" t="inlineStr">
+        <is>
+          <t>PEMADE DUNG1 MUTED</t>
+        </is>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>PEMADE DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>PEMADE DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="W143" t="inlineStr">
+        <is>
+          <t>PEMADE DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="X143" t="inlineStr">
+        <is>
+          <t>PEMADE DING2 MUTED</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" s="1" t="inlineStr">
+        <is>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>75-75</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>76-76</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>77-77</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>78-78</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>79-79</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>80-80</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>81-81</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>82-82</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>83-83</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>84-84</t>
+        </is>
+      </c>
+      <c r="O144" t="inlineStr">
+        <is>
+          <t>85-85</t>
+        </is>
+      </c>
+      <c r="P144" t="inlineStr">
+        <is>
+          <t>86-86</t>
+        </is>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>87-87</t>
+        </is>
+      </c>
+      <c r="R144" t="inlineStr">
+        <is>
+          <t>88-88</t>
+        </is>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>89-89</t>
+        </is>
+      </c>
+      <c r="T144" t="inlineStr">
+        <is>
+          <t>90-90</t>
+        </is>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>91-91</t>
+        </is>
+      </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>92-92</t>
+        </is>
+      </c>
+      <c r="W144" t="inlineStr">
+        <is>
+          <t>93-93</t>
+        </is>
+      </c>
+      <c r="X144" t="inlineStr">
+        <is>
+          <t>94-94</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" s="1" t="inlineStr">
+        <is>
+          <t>Root Key</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="n">
+        <v>75</v>
+      </c>
+      <c r="F145" t="n">
+        <v>76</v>
+      </c>
+      <c r="G145" t="n">
+        <v>77</v>
+      </c>
+      <c r="H145" t="n">
+        <v>78</v>
+      </c>
+      <c r="I145" t="n">
+        <v>79</v>
+      </c>
+      <c r="J145" t="n">
+        <v>80</v>
+      </c>
+      <c r="K145" t="n">
+        <v>81</v>
+      </c>
+      <c r="L145" t="n">
+        <v>82</v>
+      </c>
+      <c r="M145" t="n">
+        <v>83</v>
+      </c>
+      <c r="N145" t="n">
+        <v>84</v>
+      </c>
+      <c r="O145" t="n">
+        <v>85</v>
+      </c>
+      <c r="P145" t="n">
+        <v>86</v>
+      </c>
+      <c r="Q145" t="n">
+        <v>87</v>
+      </c>
+      <c r="R145" t="n">
+        <v>88</v>
+      </c>
+      <c r="S145" t="n">
+        <v>89</v>
+      </c>
+      <c r="T145" t="n">
+        <v>90</v>
+      </c>
+      <c r="U145" t="n">
+        <v>91</v>
+      </c>
+      <c r="V145" t="n">
+        <v>92</v>
+      </c>
+      <c r="W145" t="n">
+        <v>93</v>
+      </c>
+      <c r="X145" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>REYONG</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>REYONG DENG0 OPEN</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>REYONG DUNG0 OPEN</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>REYONG DANG0 OPEN</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>REYONG DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>REYONG DENGDIN0 OPEN</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>REYONG DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>REYONG DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>REYONG DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>REYONG DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>REYONG DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="O147" t="inlineStr">
+        <is>
+          <t>REYONG DONG2 OPEN</t>
+        </is>
+      </c>
+      <c r="P147" t="inlineStr">
+        <is>
+          <t>REYONG DENG2 OPEN</t>
+        </is>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>REYONG DUNG2 OPEN</t>
+        </is>
+      </c>
+      <c r="R147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG MUTED</t>
+        </is>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG MUTED</t>
+        </is>
+      </c>
+      <c r="T147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG MUTED</t>
+        </is>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG MUTED</t>
+        </is>
+      </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG OPEN</t>
+        </is>
+      </c>
+      <c r="W147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG OPEN</t>
+        </is>
+      </c>
+      <c r="X147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG OPEN</t>
+        </is>
+      </c>
+      <c r="Y147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG OPEN</t>
+        </is>
+      </c>
+      <c r="Z147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG ABBREVI</t>
+        </is>
+      </c>
+      <c r="AA147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG ABBREVI</t>
+        </is>
+      </c>
+      <c r="AB147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG ABBREVI</t>
+        </is>
+      </c>
+      <c r="AC147" t="inlineStr">
+        <is>
+          <t>REYONG BYONG ABBREVI</t>
+        </is>
+      </c>
+      <c r="AD147" t="inlineStr">
+        <is>
+          <t>REYONG TICK OPEN</t>
+        </is>
+      </c>
+      <c r="AE147" t="inlineStr">
+        <is>
+          <t>REYONG TICK_2_P OPEN</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" s="1" t="inlineStr">
+        <is>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>30-30</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>31-31</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>32-32</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>33-33</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>34-34</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>35-35</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>36-36</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>37-37</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>38-38</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>39-39</t>
+        </is>
+      </c>
+      <c r="O148" t="inlineStr">
+        <is>
+          <t>40-40</t>
+        </is>
+      </c>
+      <c r="P148" t="inlineStr">
+        <is>
+          <t>41-41</t>
+        </is>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>42-42</t>
+        </is>
+      </c>
+      <c r="R148" t="inlineStr">
+        <is>
+          <t>43-43</t>
+        </is>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>43-43</t>
+        </is>
+      </c>
+      <c r="T148" t="inlineStr">
+        <is>
+          <t>43-43</t>
+        </is>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>43-43</t>
+        </is>
+      </c>
+      <c r="V148" t="inlineStr">
+        <is>
+          <t>44-44</t>
+        </is>
+      </c>
+      <c r="W148" t="inlineStr">
+        <is>
+          <t>44-44</t>
+        </is>
+      </c>
+      <c r="X148" t="inlineStr">
+        <is>
+          <t>44-44</t>
+        </is>
+      </c>
+      <c r="Y148" t="inlineStr">
+        <is>
+          <t>44-44</t>
+        </is>
+      </c>
+      <c r="Z148" t="inlineStr">
+        <is>
+          <t>45-45</t>
+        </is>
+      </c>
+      <c r="AA148" t="inlineStr">
+        <is>
+          <t>45-45</t>
+        </is>
+      </c>
+      <c r="AB148" t="inlineStr">
+        <is>
+          <t>45-45</t>
+        </is>
+      </c>
+      <c r="AC148" t="inlineStr">
+        <is>
+          <t>45-45</t>
+        </is>
+      </c>
+      <c r="AD148" t="inlineStr">
+        <is>
+          <t>46-46</t>
+        </is>
+      </c>
+      <c r="AE148" t="inlineStr">
+        <is>
+          <t>47-47</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" s="1" t="inlineStr">
+        <is>
+          <t>Root Key</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="n">
+        <v>30</v>
+      </c>
+      <c r="F149" t="n">
+        <v>31</v>
+      </c>
+      <c r="G149" t="n">
+        <v>32</v>
+      </c>
+      <c r="H149" t="n">
+        <v>33</v>
+      </c>
+      <c r="I149" t="n">
+        <v>34</v>
+      </c>
+      <c r="J149" t="n">
+        <v>35</v>
+      </c>
+      <c r="K149" t="n">
+        <v>36</v>
+      </c>
+      <c r="L149" t="n">
+        <v>37</v>
+      </c>
+      <c r="M149" t="n">
+        <v>38</v>
+      </c>
+      <c r="N149" t="n">
+        <v>39</v>
+      </c>
+      <c r="O149" t="n">
+        <v>40</v>
+      </c>
+      <c r="P149" t="n">
+        <v>41</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>42</v>
+      </c>
+      <c r="R149" t="n">
+        <v>43</v>
+      </c>
+      <c r="S149" t="n">
+        <v>43</v>
+      </c>
+      <c r="T149" t="n">
+        <v>43</v>
+      </c>
+      <c r="U149" t="n">
+        <v>43</v>
+      </c>
+      <c r="V149" t="n">
+        <v>44</v>
+      </c>
+      <c r="W149" t="n">
+        <v>44</v>
+      </c>
+      <c r="X149" t="n">
+        <v>44</v>
+      </c>
+      <c r="Y149" t="n">
+        <v>44</v>
+      </c>
+      <c r="Z149" t="n">
+        <v>45</v>
+      </c>
+      <c r="AA149" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB149" t="n">
+        <v>45</v>
+      </c>
+      <c r="AC149" t="n">
+        <v>45</v>
+      </c>
+      <c r="AD149" t="n">
+        <v>46</v>
+      </c>
+      <c r="AE149" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>UGAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" s="1" t="inlineStr">
+        <is>
+          <t>Sample name</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>UGAL DONG0 OPEN</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>UGAL DONG0 MUTED</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>UGAL DENG0 OPEN</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>UGAL DENG0 MUTED</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>UGAL DUNG0 OPEN</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>UGAL DUNG0 MUTED</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>UGAL DANG0 OPEN</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>UGAL DANG0 MUTED</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>UGAL DING1 OPEN</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>UGAL DING1 MUTED</t>
+        </is>
+      </c>
+      <c r="O151" t="inlineStr">
+        <is>
+          <t>UGAL DONG1 OPEN</t>
+        </is>
+      </c>
+      <c r="P151" t="inlineStr">
+        <is>
+          <t>UGAL DONG1 MUTED</t>
+        </is>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>UGAL DENG1 OPEN</t>
+        </is>
+      </c>
+      <c r="R151" t="inlineStr">
+        <is>
+          <t>UGAL DENG1 MUTED</t>
+        </is>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>UGAL DUNG1 OPEN</t>
+        </is>
+      </c>
+      <c r="T151" t="inlineStr">
+        <is>
+          <t>UGAL DUNG1 MUTED</t>
+        </is>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>UGAL DANG1 OPEN</t>
+        </is>
+      </c>
+      <c r="V151" t="inlineStr">
+        <is>
+          <t>UGAL DANG1 MUTED</t>
+        </is>
+      </c>
+      <c r="W151" t="inlineStr">
+        <is>
+          <t>UGAL DING2 OPEN</t>
+        </is>
+      </c>
+      <c r="X151" t="inlineStr">
+        <is>
+          <t>UGAL DING2 MUTED</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" s="1" t="inlineStr">
+        <is>
+          <t>Key Range</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>95-95</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>95-95</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>96-96</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>96-96</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>97-97</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>97-97</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>98-98</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>98-98</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>99-99</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>99-99</t>
+        </is>
+      </c>
+      <c r="O152" t="inlineStr">
+        <is>
+          <t>100-100</t>
+        </is>
+      </c>
+      <c r="P152" t="inlineStr">
+        <is>
+          <t>100-100</t>
+        </is>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>101-101</t>
+        </is>
+      </c>
+      <c r="R152" t="inlineStr">
+        <is>
+          <t>101-101</t>
+        </is>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>102-102</t>
+        </is>
+      </c>
+      <c r="T152" t="inlineStr">
+        <is>
+          <t>102-102</t>
+        </is>
+      </c>
+      <c r="U152" t="inlineStr">
+        <is>
+          <t>103-103</t>
+        </is>
+      </c>
+      <c r="V152" t="inlineStr">
+        <is>
+          <t>103-103</t>
+        </is>
+      </c>
+      <c r="W152" t="inlineStr">
+        <is>
+          <t>104-104</t>
+        </is>
+      </c>
+      <c r="X152" t="inlineStr">
+        <is>
+          <t>104-104</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" s="1" t="inlineStr">
+        <is>
+          <t>Root Key</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="n">
+        <v>95</v>
+      </c>
+      <c r="F153" t="n">
+        <v>95</v>
+      </c>
+      <c r="G153" t="n">
+        <v>96</v>
+      </c>
+      <c r="H153" t="n">
+        <v>96</v>
+      </c>
+      <c r="I153" t="n">
+        <v>97</v>
+      </c>
+      <c r="J153" t="n">
+        <v>97</v>
+      </c>
+      <c r="K153" t="n">
+        <v>98</v>
+      </c>
+      <c r="L153" t="n">
+        <v>98</v>
+      </c>
+      <c r="M153" t="n">
+        <v>99</v>
+      </c>
+      <c r="N153" t="n">
+        <v>99</v>
+      </c>
+      <c r="O153" t="n">
+        <v>100</v>
+      </c>
+      <c r="P153" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>101</v>
+      </c>
+      <c r="R153" t="n">
+        <v>101</v>
+      </c>
+      <c r="S153" t="n">
+        <v>102</v>
+      </c>
+      <c r="T153" t="n">
+        <v>102</v>
+      </c>
+      <c r="U153" t="n">
+        <v>103</v>
+      </c>
+      <c r="V153" t="n">
+        <v>103</v>
+      </c>
+      <c r="W153" t="n">
+        <v>104</v>
+      </c>
+      <c r="X153" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n"/>
+      <c r="B154" s="2" t="n"/>
+      <c r="C154" s="2" t="n"/>
+      <c r="D154" s="2" t="n"/>
+      <c r="E154" s="2" t="n"/>
+      <c r="F154" s="2" t="n"/>
+      <c r="G154" s="2" t="n"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
+        <is>
+          <t>Presets</t>
+        </is>
+      </c>
+      <c r="B155" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C155" s="1" t="inlineStr">
+        <is>
+          <t>Generators</t>
+        </is>
+      </c>
+      <c r="D155" s="1" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="E155" s="1" t="inlineStr">
+        <is>
+          <t>Preset</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Gong Kebyar melodic</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="n">
+        <v>0</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" s="1" t="inlineStr">
+        <is>
           <t>Instrument name</t>
         </is>
       </c>
-      <c r="D140" t="inlineStr">
+      <c r="D157" t="inlineStr">
         <is>
           <t>Global</t>
         </is>
       </c>
-      <c r="E140" t="inlineStr">
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>JEGOGAN</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>CALUNG</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>PEMADE</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>KANTILAN</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>UGAL</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>REYONG</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Gong Kebyar percussion</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="n">
+        <v>128</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" s="1" t="inlineStr">
+        <is>
+          <t>Instrument name</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Global</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
         <is>
           <t>GONGS</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr">
+      <c r="F159" t="inlineStr">
         <is>
           <t>KEMPLI</t>
         </is>
       </c>
-      <c r="G140" t="inlineStr">
+      <c r="G159" t="inlineStr">
         <is>
           <t>CENGCENG</t>
         </is>
       </c>
-      <c r="H140" t="inlineStr">
+      <c r="H159" t="inlineStr">
         <is>
           <t>KENDANG</t>
         </is>
       </c>
     </row>
-    <row r="141">
-      <c r="A141" s="1" t="inlineStr">
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
         <is>
           <t>End of data</t>
         </is>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" s="2" t="n"/>
-      <c r="B142" s="2" t="n"/>
-      <c r="C142" s="2" t="n"/>
-      <c r="D142" s="2" t="n"/>
-      <c r="E142" s="2" t="n"/>
-      <c r="F142" s="2" t="n"/>
-      <c r="G142" s="2" t="n"/>
+    <row r="161">
+      <c r="A161" s="2" t="n"/>
+      <c r="B161" s="2" t="n"/>
+      <c r="C161" s="2" t="n"/>
+      <c r="D161" s="2" t="n"/>
+      <c r="E161" s="2" t="n"/>
+      <c r="F161" s="2" t="n"/>
+      <c r="G161" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>